<commit_message>
Added workflow for Data table Manipulations
</commit_message>
<xml_diff>
--- a/panDetail.xlsx
+++ b/panDetail.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RPA_UI_PATH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0599D01E-561E-435C-91FE-CE5AD924FDF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D238BECF-8312-4B77-BC8A-F1737212C409}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8964" xr2:uid="{7F97C75D-3D20-425E-AACA-EECB256DE0BA}"/>
   </bookViews>
@@ -30,7 +30,14 @@
     <t>PAN NUMBERS</t>
   </si>
   <si>
-    <t xml:space="preserve">PAN NO.AAACS8577K _x000D_
+    <t xml:space="preserve">This is to Certify that DEO PRASAD SHAW AND BAIJNATH SHAW (LOAN Account _x000D_
+Number 35569810055 ) has/have been granted a Housing Loan of Rs.10,00,000.00 _x000D_
+@08.35% annum (Floating Rate ofInterest ). _x000D_
+_x000D_
+The above loan is repayable in Equated Monthly Instalments ( EMI ) comprising Principal _x000D_
+and Interest .The Total amount of EMIs payable from 01.04.2018 to 31.03.2019 is Rs. _x000D_
+152088/The _x000D_
+break up ofthe amount into Principal &amp;Interestis given below._x000D_
 _x000D_
 </t>
   </si>
@@ -412,7 +419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>

</xml_diff>